<commit_message>
Restored from revision #96375d3c71118569013730d9a2cabe9127770db1.TEST Author: admin. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/Sample Project/Main.xlsx
+++ b/DESIGN/rules/Sample Project/Main.xlsx
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Rule</t>
   </si>
@@ -258,9 +258,6 @@
   </si>
   <si>
     <t>Rules String Hello (Integer hour)</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
 </sst>
 </file>
@@ -1075,8 +1072,8 @@
       <c r="B10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="20">
-        <v>18</v>
+      <c r="C10" s="20" t="n">
+        <v>1.0</v>
       </c>
       <c r="D10" s="21">
         <v>21</v>
@@ -1087,7 +1084,7 @@
     </row>
     <row r="11" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C11" s="24">
         <v>22</v>

</xml_diff>

<commit_message>
Restored from revision #097950a3f594f6bf2ff07f8d9a949f5215fe72f4.TEST Author: admin. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/Sample Project/Main.xlsx
+++ b/DESIGN/rules/Sample Project/Main.xlsx
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Rule</t>
   </si>
@@ -258,9 +258,6 @@
   </si>
   <si>
     <t>Rules String Hello (Integer hour)</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
 </sst>
 </file>
@@ -1075,8 +1072,8 @@
       <c r="B10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="20">
-        <v>18</v>
+      <c r="C10" s="20" t="n">
+        <v>1.0</v>
       </c>
       <c r="D10" s="21">
         <v>21</v>
@@ -1087,7 +1084,7 @@
     </row>
     <row r="11" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C11" s="24">
         <v>22</v>

</xml_diff>

<commit_message>
Restored from revision #e784a9f43386624c2f6a5935a63d60f67635f89b.TEST Author: admin. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/Sample Project/Main.xlsx
+++ b/DESIGN/rules/Sample Project/Main.xlsx
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Rule</t>
   </si>
@@ -258,9 +258,6 @@
   </si>
   <si>
     <t>Rules String Hello (Integer hour)</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
 </sst>
 </file>
@@ -1075,8 +1072,8 @@
       <c r="B10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="20">
-        <v>18</v>
+      <c r="C10" s="20" t="n">
+        <v>1.0</v>
       </c>
       <c r="D10" s="21">
         <v>21</v>
@@ -1087,7 +1084,7 @@
     </row>
     <row r="11" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C11" s="24">
         <v>22</v>

</xml_diff>

<commit_message>
Restored from revision #d73b50c9ff40270c427633de6fd052d2b27e2746.TEST Author: admin. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/Sample Project/Main.xlsx
+++ b/DESIGN/rules/Sample Project/Main.xlsx
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Rule</t>
   </si>
@@ -258,9 +258,6 @@
   </si>
   <si>
     <t>Rules String Hello (Integer hour)</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
 </sst>
 </file>
@@ -1075,8 +1072,8 @@
       <c r="B10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="20">
-        <v>18</v>
+      <c r="C10" s="20" t="n">
+        <v>1.0</v>
       </c>
       <c r="D10" s="21">
         <v>21</v>
@@ -1087,7 +1084,7 @@
     </row>
     <row r="11" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C11" s="24">
         <v>22</v>

</xml_diff>

<commit_message>
Restored from revision #ae04f7c0315726d273de4c9ef8d7dc34be60db6d.TEST Author: admin. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/Sample Project/Main.xlsx
+++ b/DESIGN/rules/Sample Project/Main.xlsx
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Rule</t>
   </si>
@@ -258,9 +258,6 @@
   </si>
   <si>
     <t>Rules String Hello (Integer hour)</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
 </sst>
 </file>
@@ -1075,8 +1072,8 @@
       <c r="B10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="20">
-        <v>18</v>
+      <c r="C10" s="20" t="n">
+        <v>1.0</v>
       </c>
       <c r="D10" s="21">
         <v>21</v>
@@ -1087,7 +1084,7 @@
     </row>
     <row r="11" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C11" s="24">
         <v>22</v>

</xml_diff>